<commit_message>
plan de vuelo en estructuras
</commit_message>
<xml_diff>
--- a/IAPs.xlsx
+++ b/IAPs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verti\Desktop\misilnl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485BCAE3-2347-4B73-A03D-ED8D7FB05E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C52BBB6-35A3-4C5C-9F5D-EA75C48CDE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10284" yWindow="1512" windowWidth="11520" windowHeight="10428" xr2:uid="{5AAB4D9E-7DEC-4EF0-B3B6-FD19669AD4F3}"/>
+    <workbookView xWindow="4224" yWindow="3480" windowWidth="17280" windowHeight="8964" xr2:uid="{5AAB4D9E-7DEC-4EF0-B3B6-FD19669AD4F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Airport</t>
   </si>
@@ -49,24 +49,6 @@
   </si>
   <si>
     <t>Altitude</t>
-  </si>
-  <si>
-    <t>KSEA</t>
-  </si>
-  <si>
-    <t>RNAVZRWY34L</t>
-  </si>
-  <si>
-    <t>34L</t>
-  </si>
-  <si>
-    <t>BAKMN</t>
-  </si>
-  <si>
-    <t>JALON</t>
-  </si>
-  <si>
-    <t>RW34L</t>
   </si>
   <si>
     <t>Latitude</t>
@@ -432,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F2BA84-1869-4E23-A80A-FA6104C1CC6B}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,30 +437,30 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
+      <c r="C2">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>36</v>
       </c>
       <c r="E2">
         <v>3000</v>
@@ -497,8 +479,17 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
-        <v>9</v>
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>37</v>
       </c>
       <c r="E3">
         <v>2400</v>
@@ -517,8 +508,17 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>10</v>
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>38</v>
       </c>
       <c r="E4">
         <v>433</v>

</xml_diff>